<commit_message>
Saving some useless models for comparison
</commit_message>
<xml_diff>
--- a/data/g_vs_random.xlsx
+++ b/data/g_vs_random.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>54.7</v>
+        <v>54.6</v>
       </c>
       <c r="C2" t="n">
-        <v>23.746</v>
+        <v>24.165</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>53.4</v>
+        <v>56.8</v>
       </c>
       <c r="C3" t="n">
-        <v>24.5</v>
+        <v>23.607</v>
       </c>
     </row>
     <row r="4">
@@ -478,10 +478,23 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>54.4</v>
+        <v>52.7</v>
       </c>
       <c r="C4" t="n">
-        <v>23.78</v>
+        <v>24.649</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>56.2</v>
+      </c>
+      <c r="C5" t="n">
+        <v>23.398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Perverse rewards show no effect!
</commit_message>
<xml_diff>
--- a/data/g_vs_random.xlsx
+++ b/data/g_vs_random.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>54.6</v>
+        <v>51.4</v>
       </c>
       <c r="C2" t="n">
-        <v>24.165</v>
+        <v>24.417</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>56.8</v>
+        <v>54.8</v>
       </c>
       <c r="C3" t="n">
-        <v>23.607</v>
+        <v>24.108</v>
       </c>
     </row>
     <row r="4">
@@ -478,10 +478,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>52.7</v>
+        <v>50.8</v>
       </c>
       <c r="C4" t="n">
-        <v>24.649</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="5">
@@ -491,10 +491,62 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>56.2</v>
+        <v>54.5</v>
       </c>
       <c r="C5" t="n">
-        <v>23.398</v>
+        <v>23.945</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>55.7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>24.47</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>24.002</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>52.3</v>
+      </c>
+      <c r="C8" t="n">
+        <v>24.369</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>55</v>
+      </c>
+      <c r="C9" t="n">
+        <v>24.221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>